<commit_message>
iOS and Android Fix
</commit_message>
<xml_diff>
--- a/iOSratings.xlsx
+++ b/iOSratings.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,7 +478,7 @@
         <v>4.8</v>
       </c>
       <c r="E2" t="n">
-        <v>59459</v>
+        <v>60564</v>
       </c>
       <c r="F2" t="inlineStr"/>
     </row>
@@ -488,7 +488,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -500,7 +500,7 @@
         <v>4.8</v>
       </c>
       <c r="E3" t="n">
-        <v>4133</v>
+        <v>4256</v>
       </c>
       <c r="F3" t="inlineStr"/>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -544,10 +544,10 @@
         <v>4.6</v>
       </c>
       <c r="E5" t="n">
-        <v>383747</v>
+        <v>390886</v>
       </c>
       <c r="F5" t="n">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -568,10 +568,10 @@
         <v>4.6</v>
       </c>
       <c r="E6" t="n">
-        <v>4717709</v>
+        <v>4733942</v>
       </c>
       <c r="F6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -580,7 +580,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -592,10 +592,10 @@
         <v>4.5</v>
       </c>
       <c r="E7" t="n">
-        <v>42009</v>
+        <v>42553</v>
       </c>
       <c r="F7" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
@@ -604,7 +604,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -616,7 +616,7 @@
         <v>4.6</v>
       </c>
       <c r="E8" t="n">
-        <v>316632</v>
+        <v>319482</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -638,7 +638,7 @@
         <v>4.8</v>
       </c>
       <c r="E9" t="n">
-        <v>2413697</v>
+        <v>2412896</v>
       </c>
       <c r="F9" t="n">
         <v>4</v>
@@ -650,7 +650,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -662,10 +662,10 @@
         <v>4.8</v>
       </c>
       <c r="E10" t="n">
-        <v>42682</v>
+        <v>42734</v>
       </c>
       <c r="F10" t="n">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11">
@@ -674,7 +674,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -686,10 +686,10 @@
         <v>4.7</v>
       </c>
       <c r="E11" t="n">
-        <v>23149</v>
+        <v>23993</v>
       </c>
       <c r="F11" t="n">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12">
@@ -698,7 +698,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -710,10 +710,10 @@
         <v>4.8</v>
       </c>
       <c r="E12" t="n">
-        <v>1941261</v>
+        <v>1973401</v>
       </c>
       <c r="F12" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -722,7 +722,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -734,7 +734,7 @@
         <v>4.5</v>
       </c>
       <c r="E13" t="n">
-        <v>1047340</v>
+        <v>1047459</v>
       </c>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -756,10 +756,10 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="n">
-        <v>254538</v>
+        <v>256189</v>
       </c>
       <c r="F14" t="n">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15">
@@ -768,7 +768,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -780,10 +780,10 @@
         <v>4.4</v>
       </c>
       <c r="E15" t="n">
-        <v>113626</v>
+        <v>114733</v>
       </c>
       <c r="F15" t="n">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16">
@@ -792,7 +792,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -804,10 +804,10 @@
         <v>4.4</v>
       </c>
       <c r="E16" t="n">
-        <v>68853</v>
+        <v>72015</v>
       </c>
       <c r="F16" t="n">
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17">
@@ -816,7 +816,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -828,7 +828,7 @@
         <v>4.3</v>
       </c>
       <c r="E17" t="n">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F17" t="inlineStr"/>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -850,10 +850,10 @@
         <v>4.7</v>
       </c>
       <c r="E18" t="n">
-        <v>398841</v>
+        <v>405414</v>
       </c>
       <c r="F18" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19">
@@ -862,7 +862,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -874,10 +874,10 @@
         <v>4</v>
       </c>
       <c r="E19" t="n">
-        <v>3992115</v>
+        <v>3991605</v>
       </c>
       <c r="F19" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -886,7 +886,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -898,11 +898,9 @@
         <v>4.6</v>
       </c>
       <c r="E20" t="n">
-        <v>4048</v>
-      </c>
-      <c r="F20" t="n">
-        <v>77</v>
-      </c>
+        <v>4103</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -910,7 +908,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -922,7 +920,7 @@
         <v>3.3</v>
       </c>
       <c r="E21" t="n">
-        <v>6450</v>
+        <v>6525</v>
       </c>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -932,7 +930,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -944,10 +942,10 @@
         <v>2.8</v>
       </c>
       <c r="E22" t="n">
-        <v>3008</v>
+        <v>3091</v>
       </c>
       <c r="F22" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23">
@@ -956,7 +954,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -968,10 +966,10 @@
         <v>4.4</v>
       </c>
       <c r="E23" t="n">
-        <v>44199</v>
+        <v>45091</v>
       </c>
       <c r="F23" t="n">
-        <v>153</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24">
@@ -980,7 +978,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -992,10 +990,10 @@
         <v>4.4</v>
       </c>
       <c r="E24" t="n">
-        <v>845713</v>
+        <v>860618</v>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -1004,7 +1002,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1016,7 +1014,7 @@
         <v>3.5</v>
       </c>
       <c r="E25" t="n">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -1026,7 +1024,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1038,7 +1036,7 @@
         <v>4.2</v>
       </c>
       <c r="E26" t="n">
-        <v>1523</v>
+        <v>1563</v>
       </c>
       <c r="F26" t="inlineStr"/>
     </row>
@@ -1048,7 +1046,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1057,10 +1055,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="E27" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F27" t="inlineStr"/>
     </row>
@@ -1070,7 +1068,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1092,7 +1090,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1104,7 +1102,7 @@
         <v>1.9</v>
       </c>
       <c r="E29" t="n">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="F29" t="inlineStr"/>
     </row>
@@ -1114,7 +1112,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1136,7 +1134,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1145,10 +1143,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E31" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F31" t="inlineStr"/>
     </row>
@@ -1158,7 +1156,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1170,7 +1168,7 @@
         <v>1.4</v>
       </c>
       <c r="E32" t="n">
-        <v>1348</v>
+        <v>1362</v>
       </c>
       <c r="F32" t="inlineStr"/>
     </row>
@@ -1180,7 +1178,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1192,7 +1190,7 @@
         <v>4.4</v>
       </c>
       <c r="E33" t="n">
-        <v>26421</v>
+        <v>27433</v>
       </c>
       <c r="F33" t="inlineStr"/>
     </row>
@@ -1202,20 +1200,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>My SECTV</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E34" t="n">
-        <v>43</v>
-      </c>
+          <t>App Store</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
@@ -1224,7 +1218,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1236,7 +1230,7 @@
         <v>4.6</v>
       </c>
       <c r="E35" t="n">
-        <v>12757</v>
+        <v>13130</v>
       </c>
       <c r="F35" t="inlineStr"/>
     </row>
@@ -1246,7 +1240,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1258,7 +1252,7 @@
         <v>1.3</v>
       </c>
       <c r="E36" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F36" t="inlineStr"/>
     </row>
@@ -1268,7 +1262,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1280,7 +1274,7 @@
         <v>4.6</v>
       </c>
       <c r="E37" t="n">
-        <v>3148</v>
+        <v>3215</v>
       </c>
       <c r="F37" t="inlineStr"/>
     </row>
@@ -1290,7 +1284,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2023-04-27 13:33:52</t>
+          <t>2023-05-25 13:07:26</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">

</xml_diff>

<commit_message>
Python Virtual Environment & Combined DataFrame
</commit_message>
<xml_diff>
--- a/iOSratings.xlsx
+++ b/iOSratings.xlsx
@@ -446,17 +446,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>App Rating</t>
+          <t>iOS App Rating</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Review Count</t>
+          <t>iOS Review Count</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Rank</t>
+          <t>iOS Rank</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,7 +478,7 @@
         <v>4.8</v>
       </c>
       <c r="E2" t="n">
-        <v>61732</v>
+        <v>61742</v>
       </c>
       <c r="F2" t="inlineStr"/>
     </row>
@@ -488,7 +488,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -500,7 +500,7 @@
         <v>4.8</v>
       </c>
       <c r="E3" t="n">
-        <v>4419</v>
+        <v>4426</v>
       </c>
       <c r="F3" t="inlineStr"/>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -544,10 +544,10 @@
         <v>4.6</v>
       </c>
       <c r="E5" t="n">
-        <v>398950</v>
+        <v>399031</v>
       </c>
       <c r="F5" t="n">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6">
@@ -556,7 +556,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -568,10 +568,10 @@
         <v>4.6</v>
       </c>
       <c r="E6" t="n">
-        <v>4754128</v>
+        <v>4754388</v>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -580,7 +580,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -592,7 +592,7 @@
         <v>4.5</v>
       </c>
       <c r="E7" t="n">
-        <v>43142</v>
+        <v>43149</v>
       </c>
       <c r="F7" t="n">
         <v>93</v>
@@ -604,7 +604,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -616,7 +616,7 @@
         <v>4.6</v>
       </c>
       <c r="E8" t="n">
-        <v>322205</v>
+        <v>322237</v>
       </c>
       <c r="F8" t="inlineStr"/>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -638,7 +638,7 @@
         <v>4.8</v>
       </c>
       <c r="E9" t="n">
-        <v>2412804</v>
+        <v>2412812</v>
       </c>
       <c r="F9" t="n">
         <v>4</v>
@@ -650,7 +650,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -662,10 +662,10 @@
         <v>4.8</v>
       </c>
       <c r="E10" t="n">
-        <v>42795</v>
+        <v>42796</v>
       </c>
       <c r="F10" t="n">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
@@ -674,7 +674,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -686,10 +686,10 @@
         <v>4.7</v>
       </c>
       <c r="E11" t="n">
-        <v>24949</v>
+        <v>24958</v>
       </c>
       <c r="F11" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
@@ -698,7 +698,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -710,10 +710,10 @@
         <v>4.8</v>
       </c>
       <c r="E12" t="n">
-        <v>2009585</v>
+        <v>2010064</v>
       </c>
       <c r="F12" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -722,7 +722,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -734,7 +734,7 @@
         <v>4.5</v>
       </c>
       <c r="E13" t="n">
-        <v>1047308</v>
+        <v>1047309</v>
       </c>
       <c r="F13" t="inlineStr"/>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -756,10 +756,10 @@
         <v>4.5</v>
       </c>
       <c r="E14" t="n">
-        <v>258047</v>
+        <v>258060</v>
       </c>
       <c r="F14" t="n">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15">
@@ -768,7 +768,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -780,7 +780,7 @@
         <v>4.4</v>
       </c>
       <c r="E15" t="n">
-        <v>116036</v>
+        <v>116043</v>
       </c>
       <c r="F15" t="inlineStr"/>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -802,10 +802,10 @@
         <v>4.4</v>
       </c>
       <c r="E16" t="n">
-        <v>76978</v>
+        <v>77035</v>
       </c>
       <c r="F16" t="n">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17">
@@ -814,7 +814,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -848,7 +848,7 @@
         <v>4.7</v>
       </c>
       <c r="E18" t="n">
-        <v>411555</v>
+        <v>411629</v>
       </c>
       <c r="F18" t="n">
         <v>48</v>
@@ -860,7 +860,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -872,10 +872,10 @@
         <v>4</v>
       </c>
       <c r="E19" t="n">
-        <v>3991298</v>
+        <v>3991303</v>
       </c>
       <c r="F19" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -884,7 +884,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -918,7 +918,7 @@
         <v>3.3</v>
       </c>
       <c r="E21" t="n">
-        <v>6602</v>
+        <v>6603</v>
       </c>
       <c r="F21" t="inlineStr"/>
     </row>
@@ -928,7 +928,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -943,7 +943,7 @@
         <v>3161</v>
       </c>
       <c r="F22" t="n">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23">
@@ -952,7 +952,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -964,7 +964,7 @@
         <v>4.4</v>
       </c>
       <c r="E23" t="n">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="F23" t="inlineStr"/>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -986,10 +986,10 @@
         <v>4.4</v>
       </c>
       <c r="E24" t="n">
-        <v>876771</v>
+        <v>876975</v>
       </c>
       <c r="F24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -998,7 +998,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1010,7 +1010,7 @@
         <v>3.6</v>
       </c>
       <c r="E25" t="n">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F25" t="inlineStr"/>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1064,16 +1064,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>App Store</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+          <t>Astound Mobile</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
       <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -1082,7 +1086,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1104,7 +1108,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1126,7 +1130,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1148,7 +1152,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1170,7 +1174,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1182,7 +1186,7 @@
         <v>4.4</v>
       </c>
       <c r="E33" t="n">
-        <v>28366</v>
+        <v>28371</v>
       </c>
       <c r="F33" t="inlineStr"/>
     </row>
@@ -1192,7 +1196,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1214,7 +1218,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1226,7 +1230,7 @@
         <v>4.6</v>
       </c>
       <c r="E35" t="n">
-        <v>13431</v>
+        <v>13437</v>
       </c>
       <c r="F35" t="inlineStr"/>
     </row>
@@ -1236,7 +1240,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1258,7 +1262,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1270,7 +1274,7 @@
         <v>4.6</v>
       </c>
       <c r="E37" t="n">
-        <v>3296</v>
+        <v>3298</v>
       </c>
       <c r="F37" t="inlineStr"/>
     </row>
@@ -1280,7 +1284,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2023-06-26 16:03:50</t>
+          <t>2023-06-26 18:41:30</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">

</xml_diff>

<commit_message>
database duplicates fix iOSData
</commit_message>
<xml_diff>
--- a/iOSratings.xlsx
+++ b/iOSratings.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -580,7 +580,7 @@
         <v>399238</v>
       </c>
       <c r="G5" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
@@ -591,7 +591,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -642,7 +642,7 @@
         <v>43165</v>
       </c>
       <c r="G7" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -653,7 +653,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -702,7 +702,7 @@
         <v>2412815</v>
       </c>
       <c r="G9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -713,7 +713,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -733,7 +733,7 @@
         <v>42797</v>
       </c>
       <c r="G10" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11">
@@ -744,7 +744,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -764,7 +764,7 @@
         <v>24983</v>
       </c>
       <c r="G11" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
@@ -775,7 +775,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -855,7 +855,7 @@
         <v>258123</v>
       </c>
       <c r="G14" t="n">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15">
@@ -866,7 +866,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -886,7 +886,7 @@
         <v>116079</v>
       </c>
       <c r="G15" t="n">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16">
@@ -897,7 +897,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -917,7 +917,7 @@
         <v>77175</v>
       </c>
       <c r="G16" t="n">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17">
@@ -928,7 +928,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -988,7 +988,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1008,7 +1008,7 @@
         <v>3991292</v>
       </c>
       <c r="G19" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1038,7 +1038,9 @@
       <c r="F20" t="n">
         <v>4150</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>141</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1048,7 +1050,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1077,7 +1079,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1097,7 +1099,7 @@
         <v>3129</v>
       </c>
       <c r="G22" t="n">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23">
@@ -1108,7 +1110,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1128,7 +1130,7 @@
         <v>45223</v>
       </c>
       <c r="G23" t="n">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
@@ -1139,7 +1141,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1170,7 +1172,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1199,7 +1201,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1228,7 +1230,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1257,7 +1259,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1286,7 +1288,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1315,7 +1317,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1344,7 +1346,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1373,7 +1375,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1402,7 +1404,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1431,7 +1433,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1460,7 +1462,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1489,7 +1491,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1518,7 +1520,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1547,7 +1549,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2023-06-27 20:18:12</t>
+          <t>2023-06-27 22:30:24</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">

</xml_diff>